<commit_message>
PARSER WORKING -To fix- standard unit
</commit_message>
<xml_diff>
--- a/cleaned/360_one_asset_management_portfolio.xlsx
+++ b/cleaned/360_one_asset_management_portfolio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,65 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Name of Instrument</t>
+          <t>name of instrument</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ISIN</t>
+          <t>isin</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Rating/Industry</t>
+          <t>coupon</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Yield</t>
+          <t>industry</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Quantity</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Market Value</t>
+          <t>market value (mkt)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Net Asset Value (NAV)</t>
+          <t>% to net assets (nav)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>yield</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>yield to call (ytc)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>yield to maturity (ytm)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Scheme</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>AmcName</t>
         </is>
@@ -496,21 +511,17 @@
           <t>INE041025011</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Realty</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>855507</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>855507</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>3166.5736098</t>
@@ -521,17 +532,20 @@
           <t>0.043993886126563235</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">REITInvIT Instruments        </t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>REITInvIT Instruments   NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -548,21 +562,17 @@
           <t>INE0Z8Z23013</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Construction</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>2525250</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2525250</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>2504.290425</t>
@@ -573,17 +583,20 @@
           <t>0.034792643835698224</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">REITInvIT Instruments        </t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>REITInvIT Instruments   NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -600,21 +613,17 @@
           <t>INE0CCU25019</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Realty</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>186881</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>186881</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>698.93494</t>
@@ -625,17 +634,20 @@
           <t>0.009710452984599464</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">REITInvIT Instruments        </t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>REITInvIT Instruments   NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -652,21 +664,17 @@
           <t>INE0FDU25010</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Realty</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>162789</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>162789</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>485.3228457</t>
@@ -677,17 +685,20 @@
           <t>0.006742694356533199</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">REITInvIT Instruments        </t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>REITInvIT Instruments   NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -704,21 +715,17 @@
           <t>IN0020220060</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>8000000</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>8000000</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>8241.6</t>
@@ -729,17 +736,24 @@
           <t>0.11450231593497807</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.06856</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -756,21 +770,17 @@
           <t>IN0020220102</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>3000000</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>3138.192</t>
@@ -781,17 +791,24 @@
           <t>0.043599574336126566</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.06953</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -808,21 +825,17 @@
           <t>IN0020230077</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>3000000</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>3084.639</t>
@@ -833,17 +846,24 @@
           <t>0.042855551024480056</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.06957</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -860,21 +880,17 @@
           <t>IN0020220011</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>3000000</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>3049.782</t>
@@ -885,17 +901,24 @@
           <t>0.04237127524956432</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.067484</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -912,21 +935,17 @@
           <t>INE936D07174</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>3000000</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>3000000</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>2938.467</t>
@@ -937,17 +956,24 @@
           <t>0.040824752086792274</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.0773</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -964,21 +990,17 @@
           <t>IN1520220220</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>2587.5475</t>
@@ -989,17 +1011,24 @@
           <t>0.03594935223036336</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.072314</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1016,21 +1045,17 @@
           <t>IN2120220065</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>2580.6</t>
@@ -1041,17 +1066,24 @@
           <t>0.03585282912320477</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.072315</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1068,21 +1100,17 @@
           <t>INE115A07QH6</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>2570.9325</t>
@@ -1093,17 +1121,24 @@
           <t>0.035718516472833306</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.0754</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1120,21 +1155,17 @@
           <t>INE040A08773</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>2540.8075</t>
@@ -1145,17 +1176,24 @@
           <t>0.035299983388536425</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.074983</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1172,21 +1210,17 @@
           <t>INE261F08EJ7</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
         <is>
           <t>ICRA AAA</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>2523.31</t>
@@ -1197,17 +1231,24 @@
           <t>0.035056886869283814</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.07395</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1224,21 +1265,17 @@
           <t>INE936D07182</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>2518.365</t>
@@ -1249,17 +1286,24 @@
           <t>0.034988184923994255</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.0763</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1276,21 +1320,17 @@
           <t>INE115A07QC7</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>2505.545</t>
@@ -1301,17 +1341,24 @@
           <t>0.0348100739151748</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.077</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1328,21 +1375,17 @@
           <t>INE041007159</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>2500.4875</t>
@@ -1353,17 +1396,24 @@
           <t>0.03473980898326338</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.0795</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1380,21 +1430,17 @@
           <t>INE414G07IH7</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
         <is>
           <t>CRISIL AA+</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>2490.3275</t>
@@ -1405,17 +1451,24 @@
           <t>0.0345986539247918</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.0863</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1432,21 +1485,17 @@
           <t>INE124N07747</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
         <is>
           <t>ICRA AA-</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>2488.5625</t>
@@ -1457,17 +1506,24 @@
           <t>0.034574132401346686</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.097675</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1484,21 +1540,17 @@
           <t>IN0020210244</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>2472.0325</t>
@@ -1509,17 +1561,24 @@
           <t>0.03434447756704204</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.06857</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1536,21 +1595,17 @@
           <t>IN1520220279</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>1561.272</t>
@@ -1561,17 +1616,24 @@
           <t>0.021691086658468632</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.072174</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="M22" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1588,21 +1650,17 @@
           <t>IN1520220253</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>1556.3115</t>
@@ -1613,17 +1671,24 @@
           <t>0.021622169368355613</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.07216</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1640,21 +1705,17 @@
           <t>INE121A07SD9</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
         <is>
           <t>ICRA AA+</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>1523.7</t>
@@ -1665,17 +1726,24 @@
           <t>0.021169090806412116</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.0818</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1692,21 +1760,17 @@
           <t>INE115A07QQ7</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>1510.2555</t>
@@ -1717,17 +1781,24 @@
           <t>0.02098230348518956</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0.0766</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="M25" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1744,21 +1815,17 @@
           <t>INE721A07RS6</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
         <is>
           <t>CRISIL AA+</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>1503.7305</t>
@@ -1769,17 +1836,24 @@
           <t>0.020891650261121934</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>0.08885</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="M26" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1796,21 +1870,17 @@
           <t>INE556F08KS8</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>1496.3835</t>
@@ -1821,17 +1891,24 @@
           <t>0.020789576814803954</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0.074073</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="M27" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1848,21 +1925,17 @@
           <t>INE941D07208</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
         <is>
           <t>CRISIL AAA</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>1481.928</t>
@@ -1873,17 +1946,24 @@
           <t>0.020588743453806322</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.07785</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="M28" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1900,21 +1980,17 @@
           <t>IN2120220131</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>1000000</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>1062.828</t>
@@ -1925,17 +2001,24 @@
           <t>0.014766097291853629</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>0.072434</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="M29" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -1952,21 +2035,17 @@
           <t>IN2220220189</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>1000000</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>1039.534</t>
@@ -1977,17 +2056,24 @@
           <t>0.014442468755235815</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0.072132</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="M30" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2004,21 +2090,17 @@
           <t>IN1520220246</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>661400</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>661400</t>
-        </is>
-      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>678.3993028</t>
@@ -2029,17 +2111,24 @@
           <t>0.00942514697380053</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0.071697</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="M31" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2056,21 +2145,17 @@
           <t>IN0020230085</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>500000</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>500000</t>
-        </is>
-      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>513.6725</t>
@@ -2081,17 +2166,24 @@
           <t>0.007136562182356584</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>0.068666</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="M32" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2108,21 +2200,17 @@
           <t>IN1520170144</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
         <is>
           <t>SOVEREIGN</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>500000</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>500000</t>
-        </is>
-      </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>510.3505</t>
@@ -2133,17 +2221,24 @@
           <t>0.007090408924064991</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>0.070009</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="M33" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2160,21 +2255,17 @@
           <t>INE121A07RM2</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
         <is>
           <t>ICRA AA+</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>100000</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>100000</t>
-        </is>
-      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>101.2644</t>
@@ -2185,17 +2276,24 @@
           <t>0.0014068880219576287</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments GOI4584      </t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0.0819</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Debt Instruments GOI4584 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="M34" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2213,16 +2311,12 @@
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr">
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
         <is>
           <t>1942.582</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>1942.582</t>
-        </is>
-      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>211.9472429</t>
@@ -2233,17 +2327,20 @@
           <t>0.0029446284905944643</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Corporate Debt Market Development Fund PUBA1038      </t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Corporate Debt Market Development Fund PUBA1038 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
         <is>
           <t>Dynamic Bond</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="M35" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2260,21 +2357,13 @@
           <t>INE115A07PM8</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>CRISIL AAA</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>2988.8775</t>
@@ -2285,17 +2374,24 @@
           <t>0.029194705940714702</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments       </t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>0.0774</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Debt Instruments  NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="M36" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2312,21 +2408,13 @@
           <t>INE242A08452</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>CRISIL AAA</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>2496.91</t>
@@ -2337,17 +2425,24 @@
           <t>0.024389274304627725</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments       </t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>0.0734</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Debt Instruments  NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="M37" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2364,21 +2459,13 @@
           <t>INE976I08391</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>CRISIL AAA</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>2494.14</t>
@@ -2389,17 +2476,24 @@
           <t>0.024362217546545207</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Debt Instruments       </t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>0.078301</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Debt Instruments  NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="M38" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2416,21 +2510,13 @@
           <t>INE040A16EU6</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>CARE A1+</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>4961.405</t>
@@ -2441,17 +2527,24 @@
           <t>0.04846192593299378</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>0.0728</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="M39" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2468,21 +2561,13 @@
           <t>INE562A16MR8</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>4960.425</t>
@@ -2493,17 +2578,24 @@
           <t>0.04845235350594654</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>0.072798</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="M40" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2520,21 +2612,13 @@
           <t>INE028A16HO7</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>FITCH A1+</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
           <t>4912.82</t>
@@ -2545,17 +2629,24 @@
           <t>0.04798735821045259</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0.074451</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="M41" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2572,21 +2663,13 @@
           <t>INE237A160W3</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
         <is>
           <t>4500000</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>4500000</t>
-        </is>
-      </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>4496.418</t>
@@ -2597,17 +2680,24 @@
           <t>0.04392003395807842</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>0.0727495</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="M42" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2624,21 +2714,13 @@
           <t>INE160A16QQ4</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
         <is>
           <t>4500000</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>4500000</t>
-        </is>
-      </c>
       <c r="F43" t="inlineStr">
         <is>
           <t>4451.922</t>
@@ -2649,17 +2731,24 @@
           <t>0.043485406699002714</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0.072999</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="M43" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2676,21 +2765,13 @@
           <t>INE556F16AQ6</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F44" t="inlineStr">
         <is>
           <t>2497.025</t>
@@ -2701,17 +2782,24 @@
           <t>0.02439039759963837</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>0.0725</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="M44" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2728,21 +2816,13 @@
           <t>INE028A16GG5</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>FITCH A1+</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>2485.1725</t>
@@ -2753,17 +2833,24 @@
           <t>0.02427462495517157</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>0.072594</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="M45" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2780,21 +2867,13 @@
           <t>INE261F16850</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>2477.64</t>
@@ -2805,17 +2884,24 @@
           <t>0.024201049131974253</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0.073201</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="M46" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2832,21 +2918,13 @@
           <t>INE562A16NS4</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>2476.815</t>
@@ -2857,17 +2935,24 @@
           <t>0.024192990711245706</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0.072699</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="M47" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2884,21 +2969,13 @@
           <t>INE040A16GC9</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>CARE A1+</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>2474.825</t>
@@ -2909,17 +2986,24 @@
           <t>0.024173552823670178</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0.0728</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="M48" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2936,21 +3020,13 @@
           <t>INE238AD6AJ8</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>2454.5775</t>
@@ -2961,17 +3037,24 @@
           <t>0.023975779643426218</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0.07505</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="M49" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -2988,21 +3071,13 @@
           <t>INE476A16YV8</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
         <is>
           <t>2000000</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>2000000</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>1999.266</t>
@@ -3013,17 +3088,24 @@
           <t>0.019528395850036986</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Certificate of Deposit INBK441      </t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>0.066932</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Certificate of Deposit INBK441 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="M50" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3040,21 +3122,13 @@
           <t>INE860H142X6</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>ICRA A1+</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>4961.85</t>
@@ -3065,17 +3139,24 @@
           <t>0.04846627259629585</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0.075848</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="M51" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3092,21 +3173,13 @@
           <t>INE261F14MS9</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>ICRA A1+</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F52" t="inlineStr">
         <is>
           <t>4924.115</t>
@@ -3117,17 +3190,24 @@
           <t>0.048097685316063434</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>0.075</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="M52" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3144,21 +3224,13 @@
           <t>INE296A14ZI9</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>4921.72</t>
@@ -3169,17 +3241,24 @@
           <t>0.04807429147649389</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>0.07845</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="M53" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3196,21 +3275,13 @@
           <t>INE498L14BD0</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>ICRA A1+</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>2488.11</t>
@@ -3221,17 +3292,24 @@
           <t>0.02430331781685655</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0.075844</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="M54" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3248,21 +3326,13 @@
           <t>INE860H143M7</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>ICRA A1+</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F55" t="inlineStr">
         <is>
           <t>2487.57</t>
@@ -3273,17 +3343,24 @@
           <t>0.024298043214197863</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="M55" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3300,21 +3377,13 @@
           <t>INE053F14237</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F56" t="inlineStr">
         <is>
           <t>2477.7625</t>
@@ -3325,17 +3394,24 @@
           <t>0.02420224568535516</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0.0727995</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J56" t="inlineStr">
+      <c r="M56" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3352,21 +3428,13 @@
           <t>INE115A14EX5</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>ICRA A1+</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>2476.18</t>
@@ -3377,17 +3445,24 @@
           <t>0.0241867881692304</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0.073153</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="M57" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3404,21 +3479,13 @@
           <t>INE296A14XX3</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>ICRA A1+</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>2460.34</t>
@@ -3429,17 +3496,24 @@
           <t>0.024032066491242284</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>0.078449</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="M58" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3456,21 +3530,13 @@
           <t>INE233A14Y48</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>CRISIL A1+</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F59" t="inlineStr">
         <is>
           <t>2459.0975</t>
@@ -3481,17 +3547,24 @@
           <t>0.024019930021235956</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Commercial Paper HDBF332      </t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0.076849</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Commercial Paper HDBF332 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J59" t="inlineStr">
+      <c r="M59" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3508,21 +3581,13 @@
           <t>IN002024X375</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>SOVEREIGN</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
         <is>
           <t>7500000</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>7500000</t>
-        </is>
-      </c>
       <c r="F60" t="inlineStr">
         <is>
           <t>7438.4625</t>
@@ -3533,17 +3598,24 @@
           <t>0.07265728533154454</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Treasury Bill TBIL2264      </t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>0.064251</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Treasury Bill TBIL2264 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
+      <c r="M60" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3560,21 +3632,13 @@
           <t>IN002024X383</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>SOVEREIGN</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
         <is>
           <t>5000000</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>5000000</t>
-        </is>
-      </c>
       <c r="F61" t="inlineStr">
         <is>
           <t>4952.055</t>
@@ -3585,17 +3649,24 @@
           <t>0.04837059716473691</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Treasury Bill TBIL2264      </t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>0.064252</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Treasury Bill TBIL2264 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J61" t="inlineStr">
+      <c r="M61" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3612,21 +3683,13 @@
           <t>IN002024Z016</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>SOVEREIGN</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F62" t="inlineStr">
         <is>
           <t>2472.8475</t>
@@ -3637,17 +3700,24 @@
           <t>0.024154237033378417</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Treasury Bill TBIL2264      </t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>0.0657</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Treasury Bill TBIL2264 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J62" t="inlineStr">
+      <c r="M62" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3664,21 +3734,13 @@
           <t>IN002024X409</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>SOVEREIGN</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F63" t="inlineStr">
         <is>
           <t>2469.99</t>
@@ -3689,17 +3751,24 @@
           <t>0.02412632559430954</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Treasury Bill TBIL2264      </t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>0.065219</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Treasury Bill TBIL2264 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="M63" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3716,21 +3785,13 @@
           <t>IN002024Y274</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>SOVEREIGN</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
         <is>
           <t>2500000</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>2500000</t>
-        </is>
-      </c>
       <c r="F64" t="inlineStr">
         <is>
           <t>2466.9625</t>
@@ -3741,17 +3802,24 @@
           <t>0.024096753632181445</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Treasury Bill TBIL2264      </t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>0.065175</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Treasury Bill TBIL2264 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J64" t="inlineStr">
+      <c r="M64" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3768,21 +3836,13 @@
           <t>IN002024Y209</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>SOVEREIGN</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
         <is>
           <t>1500000</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>1500000</t>
-        </is>
-      </c>
       <c r="F65" t="inlineStr">
         <is>
           <t>1496.577</t>
@@ -3793,17 +3853,24 @@
           <t>0.014618238931718342</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Treasury Bill TBIL2264      </t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>0.064232</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Treasury Bill TBIL2264 NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="M65" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>
@@ -3821,16 +3888,12 @@
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
         <is>
           <t>2387.533</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>2387.533</t>
-        </is>
-      </c>
       <c r="F66" t="inlineStr">
         <is>
           <t>260.4940418</t>
@@ -3841,17 +3904,20 @@
           <t>0.0025444491952779074</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Corporate Debt Market Development Fund       </t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Corporate Debt Market Development Fund  NAN nan nan nan nan nan</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
         <is>
           <t>Liquid Fund</t>
         </is>
       </c>
-      <c r="J66" t="inlineStr">
+      <c r="M66" t="inlineStr">
         <is>
           <t>360 One Asset Management</t>
         </is>

</xml_diff>